<commit_message>
feat: add "content" email
</commit_message>
<xml_diff>
--- a/outputExcel/news.xlsx
+++ b/outputExcel/news.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ex de mulher sequestrada junto com Marcelinho teme ser atacado na rua</t>
+          <t>Ex de mulher sequestrada com Marcelinho teme ser atacado na rua</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -691,17 +691,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Vendas do PS5 ultrapassam 50 milhões de unidades, diz Sony</t>
+          <t>Lutador do UFC agradece rival por parar golpes: “Poderia ter me matado”</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/economia/vendas-do-ps5-ultrapassam-50-milhoes-de-unidades-diz-sony/</t>
+          <t>https://www.cnnbrasil.com.br/noticias/lutador-do-ufc-agradece-rival-por-parar-golpes-poderia-ter-me-matado/</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Faustão diz que pode voltar à TV em março se cuidar da saúde</t>
+          <t>Estados desistem de aumentar ICMS após mudança na reforma tributária</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/entretenimento/faustao-diz-que-pode-voltar-a-tv-em-marco-se-cuidar-da-saude/</t>
+          <t>https://www.cnnbrasil.com.br/economia/estados-desistem-de-aumentar-icms-apos-mudanca-na-reforma-tributaria/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Em reunião, Lula cobra celeridade em programas e diálogo com Congresso</t>
+          <t>Vendas do PS5 ultrapassam 50 milhões de unidades, diz Sony</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/politica/em-reuniao-lula-cobra-celeridade-em-programas-e-dialogo-com-congresso/</t>
+          <t>https://www.cnnbrasil.com.br/economia/vendas-do-ps5-ultrapassam-50-milhoes-de-unidades-diz-sony/</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20/12/2023 15:54:40</t>
+          <t>20/12/2023 16:05:59</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add message email, and finishing email sender
</commit_message>
<xml_diff>
--- a/outputExcel/news.xlsx
+++ b/outputExcel/news.xlsx
@@ -466,17 +466,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sessão tem presença de Lula e presidentes dos outros poderes</t>
+          <t>IVA, cashback, 'imposto do pecado': a reforma em 7 pontos</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2023/12/20/congresso-faz-sessao-para-promulgar-a-reforma-tributaria-com-a-presenca-dos-presidentes-dos-tres-poderes.ghtml</t>
+          <t>https://g1.globo.com/politica/noticia/2023/12/15/entenda-em-7-pontos-a-reforma-tributaria.ghtml</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -491,17 +491,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>STJ quebra sigilos de Cláudio Castro após operação contra irmão</t>
+          <t xml:space="preserve">Senado aprova medida que muda regras de descontos do ICMS </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/rj/rio-de-janeiro/noticia/2023/12/20/stj-quebra-sigilos-bancarios-e-telefonico-de-claudio-castro-e-pf-encontra-na-casa-do-irmao-dinheiro-em-caixa-de-remedios.ghtml</t>
+          <t>https://g1.globo.com/politica/noticia/2023/12/20/senado-aprova-texto-base-de-mp-que-muda-regras-de-descontos-do-icms-para-aumentar-arrecadacao-federal.ghtml</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ex de mulher sequestrada com Marcelinho teme ser atacado na rua</t>
+          <t>STJ quebra sigilos de Cláudio Castro após operação contra irmão</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/sp/sao-paulo/noticia/2023/12/20/vida-virou-do-avesso-pessoas-me-xingando-falando-que-mandei-sequestrar-diz-ex-marido-de-amiga-de-marcelinho-carioca-levada-a-cativeiro.ghtml</t>
+          <t>https://g1.globo.com/rj/rio-de-janeiro/noticia/2023/12/20/stj-quebra-sigilos-bancarios-e-telefonico-de-claudio-castro-e-pf-encontra-na-casa-do-irmao-dinheiro-em-caixa-de-remedios.ghtml</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>STJ autoriza quebra de sigilo bancário de governador do RJ a pedido da PF</t>
+          <t>Deputado do PT bate na cara de colega e usa termo homofóbico contra Nikolas</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://noticias.uol.com.br/politica/ultimas-noticias/2023/12/20/quebra-de-sigilo-bancario-claudio-castro.htm</t>
+          <t>https://noticias.uol.com.br/politica/ultimas-noticias/2023/12/20/vice-presidente-do-pt-da-tapa-na-cara-de-deputado-durante-sessao.htm</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Toffoli suspende multa bilionária da J&amp;F; esposa do ministro é advogada do grupo</t>
+          <t>Senado aprova por 48 votos a 22 proposta de Haddad para elevar arrecadação</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://piaui.folha.uol.com.br/toffoli-suspende-multa-bilionaria-do-acorde-de-leniencia-da-jf/</t>
+          <t>https://economia.uol.com.br/noticias/redacao/2023/12/20/senado-mp-subvencao-beneficios-fiscais.htm</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -591,17 +591,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Argentina instala aviso em metrô contra manifestações: 'Quem bloqueia não recebe'</t>
+          <t>Apesar de ameaças de Milei, argentinos protestam contra novo governo</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://noticias.uol.com.br/internacional/ultimas-noticias/2023/12/20/argentina-avisos-contra-manifestantes-corte-de-beneficios.htm</t>
+          <t>https://noticias.uol.com.br/internacional/ultimas-noticias/2023/12/20/protesto-contra-milei-argentina-nas-ruas-apos-ameacas.htm</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -691,17 +691,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lutador do UFC agradece rival por parar golpes: “Poderia ter me matado”</t>
+          <t>Regulamentação de cigarros eletrônicos está em discussão no Brasil</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/noticias/lutador-do-ufc-agradece-rival-por-parar-golpes-poderia-ter-me-matado/</t>
+          <t>https://www.cnnbrasil.com.br/nacional/regulamentacao-de-cigarros-eletronicos-esta-em-discussao-no-brasil/</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Estados desistem de aumentar ICMS após mudança na reforma tributária</t>
+          <t>Lula deve passar Réveillon no litoral do Rio de Janeiro</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/economia/estados-desistem-de-aumentar-icms-apos-mudanca-na-reforma-tributaria/</t>
+          <t>https://www.cnnbrasil.com.br/politica/lula-deve-passar-reveillon-no-litoral-do-rio-de-janeiro/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Vendas do PS5 ultrapassam 50 milhões de unidades, diz Sony</t>
+          <t>STJ autoriza quebra de sigilos fiscal e telemático de Cláudio Castro</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/economia/vendas-do-ps5-ultrapassam-50-milhoes-de-unidades-diz-sony/</t>
+          <t>https://www.cnnbrasil.com.br/politica/stj-autoriza-quebra-de-sigilos-fiscal-e-telematico-de-claudio-castro/</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20/12/2023 16:05:59</t>
+          <t>20/12/2023 20:17:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fix html content
</commit_message>
<xml_diff>
--- a/outputExcel/news.xlsx
+++ b/outputExcel/news.xlsx
@@ -466,17 +466,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>IVA, cashback, 'imposto do pecado': a reforma em 7 pontos</t>
+          <t>PF faz operação contra a Braskem após afundamento de solo em Maceió</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2023/12/15/entenda-em-7-pontos-a-reforma-tributaria.ghtml</t>
+          <t>https://g1.globo.com/al/alagoas/noticia/2023/12/21/pf-cumpre-mandados-em-investigacao-que-apura-crimes-cometidos-pela-braskem-em-maceio.ghtml</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -491,17 +491,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Senado aprova medida que muda regras de descontos do ICMS </t>
+          <t>Brasil reverteu 'veto' de Israel a 16 brasileiros e parentes</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/politica/noticia/2023/12/20/senado-aprova-texto-base-de-mp-que-muda-regras-de-descontos-do-icms-para-aumentar-arrecadacao-federal.ghtml</t>
+          <t>https://g1.globo.com/politica/blog/camila-bomfim/post/2023/12/21/metade-do-grupo-de-brasileiros-a-ser-repatriado-de-gaza-tinha-recebido-veto-de-israel-brasil-reverteu.ghtml</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>STJ quebra sigilos de Cláudio Castro após operação contra irmão</t>
+          <t>Milei anuncia decreto com 300 medidas para desregular economia</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://g1.globo.com/rj/rio-de-janeiro/noticia/2023/12/20/stj-quebra-sigilos-bancarios-e-telefonico-de-claudio-castro-e-pf-encontra-na-casa-do-irmao-dinheiro-em-caixa-de-remedios.ghtml</t>
+          <t>https://g1.globo.com/mundo/noticia/2023/12/20/milei-anuncia-decreto-que-estabelece-bases-para-novo-plano-economico.ghtml</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Deputado do PT bate na cara de colega e usa termo homofóbico contra Nikolas</t>
+          <t>Exploração de sal-gema pela Braskem em Maceió é alvo de operação da PF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://noticias.uol.com.br/politica/ultimas-noticias/2023/12/20/vice-presidente-do-pt-da-tapa-na-cara-de-deputado-durante-sessao.htm</t>
+          <t>https://noticias.uol.com.br/cotidiano/ultimas-noticias/2023/12/21/operacao-pf-maceio.htm</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Senado aprova por 48 votos a 22 proposta de Haddad para elevar arrecadação</t>
+          <t>Deputado chora após levar tapa na cara de colega do PT: 'Humilhado'</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://economia.uol.com.br/noticias/redacao/2023/12/20/senado-mp-subvencao-beneficios-fiscais.htm</t>
+          <t>https://noticias.uol.com.br/politica/ultimas-noticias/2023/12/20/messias-donato-pronunciamento.htm</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -591,17 +591,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Apesar de ameaças de Milei, argentinos protestam contra novo governo</t>
+          <t>Após Javier Milei anunciar megadecreto, argentinos protestam em Buenos Aires</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://noticias.uol.com.br/internacional/ultimas-noticias/2023/12/20/protesto-contra-milei-argentina-nas-ruas-apos-ameacas.htm</t>
+          <t>https://noticias.uol.com.br/internacional/ultimas-noticias/2023/12/21/apos-anuncio-de-megadecreto-argentinos-protestam-em-buenos-aires.htm</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Irmão de Cláudio Castro é alvo da PF em operação por desvios em programas sociais</t>
+          <t>Pescador captura espécie de peixe invasora que ameaça biodiversidade</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.terra.com.br/noticias/brasil/cidades/irmao-de-claudio-castro-e-alvo-da-pf-em-operacao-por-desvios-em-programas-de-assistencia-social,db25fa634369d6c354e3d0e083a7d8b20r40lefn.html</t>
+          <t>https://www.terra.com.br/planeta/noticias/pescador-captura-especie-de-peixe-invasora-que-ameaca-biodiversidade-no-rn,cb581c9e42757b17caf9bfc2d5c875346j2516sb.html</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Enfeites de Natal pesam na conta de luz? Quanto? Saiba como evitar prejuízos</t>
+          <t>Homem fatura R$ 25 milhões ajudando pessoas a comprar o presente certo</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.terra.com.br/economia/enfeites-de-natal-pesam-na-conta-de-luz-quanto-especialista-da-dicas-para-evitar-prejuizos,a43fd978f73ed6ca5e62ee8d4bba747b8a14hi8h.html</t>
+          <t>https://forbes.com.br/forbes-money/2023/12/ele-faturou-r-25-milhoes-em-2023-ajudando-pessoas-a-comprar-o-presente-certo/?utm_source=terra_capa_noticias&amp;utm_medium=referral</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -666,17 +666,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>YouTuber diz ter algemado e deixado filhos passarem fome porque estavam 'possuídos'</t>
+          <t>Governo lança nova fase de operação de repatriação de brasileiros em Gaza</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.terra.com.br/noticias/mundo/youtuber-diz-ter-algemado-e-deixado-filhos-passarem-fome-porque-estavam-possuidos,27e1c3f2850985edeea8cc18d7ed838aig8g09m5.html</t>
+          <t>https://www.terra.com.br/noticias/governo-lanca-nova-fase-de-operacao-de-repatriacao-de-brasileiros-em-gaza,5b217a63bc3016beb3c2d2e56f8e20b9xuwdzc7x.html</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -691,17 +691,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Regulamentação de cigarros eletrônicos está em discussão no Brasil</t>
+          <t>PF apreende quase 3 toneladas de drogas no Aeroporto de Guarulhos em 2023</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/nacional/regulamentacao-de-cigarros-eletronicos-esta-em-discussao-no-brasil/</t>
+          <t>https://www.cnnbrasil.com.br/nacional/pf-apreende-quase-3-toneladas-de-drogas-no-aeroporto-de-guarulhos-em-2023/</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Lula deve passar Réveillon no litoral do Rio de Janeiro</t>
+          <t>Presidente do Corinthians sobre Gabigol: “Chegaremos a um acordo”</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/politica/lula-deve-passar-reveillon-no-litoral-do-rio-de-janeiro/</t>
+          <t>https://www.cnnbrasil.com.br/esportes/presidente-do-corinthians-sobre-gabigol-chegaremos-a-um-acordo/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>STJ autoriza quebra de sigilos fiscal e telemático de Cláudio Castro</t>
+          <t>Programas de desenvolvimento humano elevam a eficiência empresarial</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.cnnbrasil.com.br/politica/stj-autoriza-quebra-de-sigilos-fiscal-e-telematico-de-claudio-castro/</t>
+          <t>https://www.cnnbrasil.com.br/branded-content/nacional/programas-de-desenvolvimento-humano-elevam-a-eficiencia-empresarial/</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20/12/2023 20:17:33</t>
+          <t>21/12/2023 09:40:13</t>
         </is>
       </c>
     </row>

</xml_diff>